<commit_message>
Updated test case data
</commit_message>
<xml_diff>
--- a/TestCasePinterest.xlsx
+++ b/TestCasePinterest.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28928"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D034C4D4-8E86-437A-9AFF-4A42B0E11503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{18E4A592-8882-4D3B-97C5-F10FCBB22471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="119">
   <si>
     <t>Project Name:</t>
   </si>
@@ -511,6 +511,10 @@
 enter username and password'</t>
   </si>
   <si>
+    <t>Error message 
+'don't forget username'</t>
+  </si>
+  <si>
     <t>TC_LOGIN_008</t>
   </si>
   <si>
@@ -608,6 +612,10 @@
       </rPr>
       <t>&lt;(blank) Password&gt;</t>
     </r>
+  </si>
+  <si>
+    <t>Error message 
+'username does not belong to an account'</t>
   </si>
   <si>
     <t>TC_LOGIN_010</t>
@@ -1229,80 +1237,6 @@
         <rFont val="Times New Roman"/>
       </rPr>
       <t>&lt;Valid 200 chars password: P@ssword123#Vx7Lp$MnZt^QwGc!RfYuHdEsKoAiJbXcNvTuMqLeWzDjBgCrFsHpYlOmTxKnVzUqAySdFgJhKlZxCvBnMqWeRtYuIoPaSdFgHjKlQwErTyUiOpAsDfGhJkLzXcVbNm&gt;</t>
-    </r>
-  </si>
-  <si>
-    <t>TC_LOGIN_026</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>Enter</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve"> valid username </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>and password that does not meet length requirement (&gt;6 chars)</t>
-    </r>
-  </si>
-  <si>
-    <t>TC_LOGIN_027</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>Enter</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>invalid username</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>and password that does not meet length requirement (&gt;6 chars)</t>
     </r>
   </si>
   <si>
@@ -1606,8 +1540,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FEDEC968-BA01-41AA-BE5A-7C5445D4FAD1}" name="Table3" displayName="Table3" ref="A7:J34" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="0">
-  <autoFilter ref="A7:J34" xr:uid="{FEDEC968-BA01-41AA-BE5A-7C5445D4FAD1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FEDEC968-BA01-41AA-BE5A-7C5445D4FAD1}" name="Table3" displayName="Table3" ref="A7:J32" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="0">
+  <autoFilter ref="A7:J32" xr:uid="{FEDEC968-BA01-41AA-BE5A-7C5445D4FAD1}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{1E7A0953-F1D9-4697-AB86-7B6A55C16511}" name="Test Case ID"/>
     <tableColumn id="2" xr3:uid="{2A8F36BC-4417-4110-A0DA-F694E9C4BF7A}" name="Test Scenario"/>
@@ -1941,10 +1875,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E7" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="D27" workbookViewId="0">
+      <selection activeCell="J32" activeCellId="1" sqref="J30 J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2246,46 +2180,54 @@
       <c r="H14" s="14" t="s">
         <v>37</v>
       </c>
+      <c r="I14" s="14" t="s">
+        <v>59</v>
+      </c>
       <c r="J14" s="21" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:10" s="11" customFormat="1" ht="45" customHeight="1">
       <c r="A15" s="11" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B15" s="12" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E15" s="13" t="s">
         <v>46</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G15" s="14" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H15" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="J15" s="21"/>
+      <c r="I15" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="J15" s="21" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="16" spans="1:10" s="11" customFormat="1" ht="45" customHeight="1">
       <c r="A16" s="11" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B16" s="12" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D16" s="17" t="s">
         <v>29</v>
@@ -2294,7 +2236,7 @@
         <v>51</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G16" s="15" t="s">
         <v>53</v>
@@ -2302,17 +2244,22 @@
       <c r="H16" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="J16" s="21"/>
+      <c r="I16" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="J16" s="21" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="17" spans="1:10" s="11" customFormat="1" ht="45" customHeight="1">
       <c r="A17" s="11" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>18</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D17" s="17" t="s">
         <v>29</v>
@@ -2321,7 +2268,7 @@
         <v>21</v>
       </c>
       <c r="F17" s="18" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G17" s="16" t="s">
         <v>23</v>
@@ -2330,7 +2277,7 @@
         <v>24</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J17" s="21" t="s">
         <v>26</v>
@@ -2338,13 +2285,13 @@
     </row>
     <row r="18" spans="1:10" s="11" customFormat="1" ht="45" customHeight="1">
       <c r="A18" s="11" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>18</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D18" s="17" t="s">
         <v>29</v>
@@ -2353,7 +2300,7 @@
         <v>21</v>
       </c>
       <c r="F18" s="17" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="G18" s="14" t="s">
         <v>31</v>
@@ -2361,17 +2308,22 @@
       <c r="H18" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="J18" s="21"/>
+      <c r="I18" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="J18" s="21" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="19" spans="1:10" s="11" customFormat="1" ht="45" customHeight="1">
       <c r="A19" s="11" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B19" s="12" t="s">
         <v>18</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D19" s="17" t="s">
         <v>29</v>
@@ -2380,7 +2332,7 @@
         <v>21</v>
       </c>
       <c r="F19" s="18" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G19" s="16" t="s">
         <v>23</v>
@@ -2397,13 +2349,13 @@
     </row>
     <row r="20" spans="1:10" s="11" customFormat="1" ht="45" customHeight="1">
       <c r="A20" s="11" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B20" s="12" t="s">
         <v>18</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D20" s="17" t="s">
         <v>29</v>
@@ -2412,7 +2364,7 @@
         <v>21</v>
       </c>
       <c r="F20" s="17" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G20" s="14" t="s">
         <v>36</v>
@@ -2420,17 +2372,22 @@
       <c r="H20" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="J20" s="21"/>
+      <c r="I20" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="J20" s="21" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="21" spans="1:10" s="11" customFormat="1" ht="45" customHeight="1">
       <c r="A21" s="11" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B21" s="12" t="s">
         <v>18</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D21" s="17" t="s">
         <v>29</v>
@@ -2439,7 +2396,7 @@
         <v>21</v>
       </c>
       <c r="F21" s="18" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G21" s="16" t="s">
         <v>23</v>
@@ -2456,13 +2413,13 @@
     </row>
     <row r="22" spans="1:10" s="11" customFormat="1" ht="45" customHeight="1">
       <c r="A22" s="11" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B22" s="12" t="s">
         <v>18</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D22" s="17" t="s">
         <v>29</v>
@@ -2471,7 +2428,7 @@
         <v>21</v>
       </c>
       <c r="F22" s="18" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G22" s="14" t="s">
         <v>31</v>
@@ -2479,17 +2436,22 @@
       <c r="H22" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="J22" s="21"/>
+      <c r="I22" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="J22" s="21" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="23" spans="1:10" s="11" customFormat="1" ht="45" customHeight="1">
       <c r="A23" s="11" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B23" s="12" t="s">
         <v>18</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D23" s="17" t="s">
         <v>29</v>
@@ -2498,7 +2460,7 @@
         <v>21</v>
       </c>
       <c r="F23" s="18" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="G23" s="16" t="s">
         <v>23</v>
@@ -2515,13 +2477,13 @@
     </row>
     <row r="24" spans="1:10" s="11" customFormat="1" ht="45" customHeight="1">
       <c r="A24" s="11" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B24" s="12" t="s">
         <v>18</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D24" s="17" t="s">
         <v>29</v>
@@ -2530,7 +2492,7 @@
         <v>21</v>
       </c>
       <c r="F24" s="17" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="G24" s="14" t="s">
         <v>36</v>
@@ -2538,17 +2500,22 @@
       <c r="H24" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="J24" s="21"/>
+      <c r="I24" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="J24" s="21" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="25" spans="1:10" s="11" customFormat="1" ht="45" customHeight="1">
       <c r="A25" s="11" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B25" s="12" t="s">
         <v>18</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D25" s="17" t="s">
         <v>29</v>
@@ -2557,7 +2524,7 @@
         <v>21</v>
       </c>
       <c r="F25" s="18" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="G25" s="16" t="s">
         <v>23</v>
@@ -2574,13 +2541,13 @@
     </row>
     <row r="26" spans="1:10" s="11" customFormat="1" ht="45" customHeight="1">
       <c r="A26" s="11" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B26" s="12" t="s">
         <v>18</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D26" s="17" t="s">
         <v>29</v>
@@ -2589,7 +2556,7 @@
         <v>21</v>
       </c>
       <c r="F26" s="18" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="G26" s="14" t="s">
         <v>31</v>
@@ -2597,17 +2564,22 @@
       <c r="H26" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="J26" s="21"/>
+      <c r="I26" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="J26" s="21" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="27" spans="1:10" s="11" customFormat="1" ht="45" customHeight="1">
       <c r="A27" s="11" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B27" s="12" t="s">
         <v>18</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D27" s="17" t="s">
         <v>29</v>
@@ -2616,7 +2588,7 @@
         <v>21</v>
       </c>
       <c r="F27" s="18" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="G27" s="16" t="s">
         <v>23</v>
@@ -2633,13 +2605,13 @@
     </row>
     <row r="28" spans="1:10" s="11" customFormat="1" ht="45" customHeight="1">
       <c r="A28" s="11" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B28" s="12" t="s">
         <v>18</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D28" s="17" t="s">
         <v>29</v>
@@ -2648,7 +2620,7 @@
         <v>21</v>
       </c>
       <c r="F28" s="17" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G28" s="14" t="s">
         <v>36</v>
@@ -2656,17 +2628,22 @@
       <c r="H28" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="J28" s="21"/>
+      <c r="I28" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="J28" s="21" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="29" spans="1:10" s="11" customFormat="1" ht="45" customHeight="1">
       <c r="A29" s="11" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B29" s="12" t="s">
         <v>18</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D29" s="17" t="s">
         <v>29</v>
@@ -2675,7 +2652,7 @@
         <v>21</v>
       </c>
       <c r="F29" s="18" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G29" s="16" t="s">
         <v>23</v>
@@ -2692,13 +2669,13 @@
     </row>
     <row r="30" spans="1:10" s="11" customFormat="1" ht="45" customHeight="1">
       <c r="A30" s="11" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B30" s="12" t="s">
         <v>18</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D30" s="17" t="s">
         <v>29</v>
@@ -2707,7 +2684,7 @@
         <v>21</v>
       </c>
       <c r="F30" s="18" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="G30" s="14" t="s">
         <v>31</v>
@@ -2715,16 +2692,22 @@
       <c r="H30" s="14" t="s">
         <v>43</v>
       </c>
+      <c r="I30" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="J30" s="21" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="31" spans="1:10" s="11" customFormat="1" ht="45" customHeight="1">
       <c r="A31" s="11" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B31" s="12" t="s">
         <v>18</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D31" s="17" t="s">
         <v>29</v>
@@ -2733,7 +2716,7 @@
         <v>21</v>
       </c>
       <c r="F31" s="18" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="G31" s="16" t="s">
         <v>23</v>
@@ -2750,13 +2733,13 @@
     </row>
     <row r="32" spans="1:10" s="11" customFormat="1" ht="45" customHeight="1">
       <c r="A32" s="11" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B32" s="12" t="s">
         <v>18</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D32" s="17" t="s">
         <v>29</v>
@@ -2765,7 +2748,7 @@
         <v>21</v>
       </c>
       <c r="F32" s="18" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="G32" s="14" t="s">
         <v>36</v>
@@ -2773,49 +2756,21 @@
       <c r="H32" s="14" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" s="11" customFormat="1" ht="45" customHeight="1">
-      <c r="A33" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="B33" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C33" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="D33" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="E33" s="13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" s="11" customFormat="1" ht="45" customHeight="1">
-      <c r="A34" s="11" t="s">
+      <c r="I32" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="J32" s="21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="7:7" s="11" customFormat="1" ht="15.75" customHeight="1">
+      <c r="G33" s="11" t="s">
         <v>118</v>
-      </c>
-      <c r="B34" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C34" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="D34" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="E34" s="13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" s="11" customFormat="1" ht="15.75" customHeight="1">
-      <c r="G35" s="11" t="s">
-        <v>120</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J7:J34" xr:uid="{62E9E32B-B07A-41C4-ADB9-49193BCD3C15}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J7:J32" xr:uid="{62E9E32B-B07A-41C4-ADB9-49193BCD3C15}">
       <formula1>"Pass,Fail"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>